<commit_message>
feat: neural networks with optimization of parameters
</commit_message>
<xml_diff>
--- a/Reports/11_Final_report_02/experiment_results.xlsx
+++ b/Reports/11_Final_report_02/experiment_results.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26408"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaspergracner/Documents/FERI_MAG/Poletni_semester/Povezljivi_sistemi_in_inteligentne_storitve/psis2017/Reports/11_Final_report/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luka/Documents/GitRepos/psis2017.git/Reports/11_Final_report_02/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-35920" yWindow="-4300" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19320" windowHeight="12800" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="neural_networks" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
   <si>
     <t>Metoda</t>
   </si>
@@ -102,6 +103,114 @@
   </si>
   <si>
     <t>0.7816</t>
+  </si>
+  <si>
+    <t>metoda</t>
+  </si>
+  <si>
+    <t>adam-identity</t>
+  </si>
+  <si>
+    <t>adam-logistic</t>
+  </si>
+  <si>
+    <t>lbfgs-logistic</t>
+  </si>
+  <si>
+    <t>adam-tanh</t>
+  </si>
+  <si>
+    <t>lbfgs-tanh</t>
+  </si>
+  <si>
+    <t>adam-relu</t>
+  </si>
+  <si>
+    <t>lbfgs-relu</t>
+  </si>
+  <si>
+    <t>lbfgs-identity</t>
+  </si>
+  <si>
+    <t>sgd-identity</t>
+  </si>
+  <si>
+    <t>sgd-tanh</t>
+  </si>
+  <si>
+    <t>sgd-relu</t>
+  </si>
+  <si>
+    <t>sgd-logistic</t>
+  </si>
+  <si>
+    <t>0.64797507788161979</t>
+  </si>
+  <si>
+    <t>0.54800000000000004</t>
+  </si>
+  <si>
+    <t>0.77551020408163263</t>
+  </si>
+  <si>
+    <t>0.69795918367346943</t>
+  </si>
+  <si>
+    <t>0.72332015810276684</t>
+  </si>
+  <si>
+    <t>0.71017274472168901</t>
+  </si>
+  <si>
+    <t>0.63752276867030966</t>
+  </si>
+  <si>
+    <t>0.61056105610561062</t>
+  </si>
+  <si>
+    <t>0.79918032786885251</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>0.6851485148514852</t>
+  </si>
+  <si>
+    <t>0.67021276595744683</t>
+  </si>
+  <si>
+    <t>0.78000000000000003</t>
+  </si>
+  <si>
+    <t>0.70399999999999996</t>
+  </si>
+  <si>
+    <t>0.71999999999999997</t>
+  </si>
+  <si>
+    <t>0.69799999999999995</t>
+  </si>
+  <si>
+    <t>0.60199999999999998</t>
+  </si>
+  <si>
+    <t>0.52800000000000002</t>
+  </si>
+  <si>
+    <t>0.80400000000000005</t>
+  </si>
+  <si>
+    <t>0.496</t>
+  </si>
+  <si>
+    <t>0.68200000000000005</t>
+  </si>
+  <si>
+    <t>0.504</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
   </si>
 </sst>
 </file>
@@ -418,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -608,4 +717,166 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.5" customWidth="1"/>
+    <col min="2" max="3" width="19.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>